<commit_message>
Se agrega una nueva hoja en el excel del reporte
</commit_message>
<xml_diff>
--- a/static/docs/layout_feria.xlsx
+++ b/static/docs/layout_feria.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\web\feria\static\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3FECA92-C9B2-4DD0-B6D7-75E098C8C542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2F0834-E6D1-4688-9D9C-5708A17A1798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="555" windowWidth="24240" windowHeight="13020" xr2:uid="{71824B8D-2F57-4AF6-8E27-099D4ACB650B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{71824B8D-2F57-4AF6-8E27-099D4ACB650B}"/>
   </bookViews>
   <sheets>
     <sheet name="LOCALES" sheetId="1" r:id="rId1"/>
+    <sheet name="MONTOS" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
   <si>
     <t>LOCAL</t>
   </si>
@@ -83,6 +84,68 @@
     <t>FERIA TABASCO 2024</t>
   </si>
   <si>
+    <t>PRODUCTOS ADICIONALES</t>
+  </si>
+  <si>
+    <t>Nave 1</t>
+  </si>
+  <si>
+    <t>Nave 3</t>
+  </si>
+  <si>
+    <t>Total de locales asignados</t>
+  </si>
+  <si>
+    <t>Total con pago confirmado</t>
+  </si>
+  <si>
+    <t>Monto total</t>
+  </si>
+  <si>
+    <t>Zona A</t>
+  </si>
+  <si>
+    <t>Zona B</t>
+  </si>
+  <si>
+    <t>Zona C</t>
+  </si>
+  <si>
+    <t>Zona D</t>
+  </si>
+  <si>
+    <t>Terrazas</t>
+  </si>
+  <si>
+    <t>Terrazas Grandes</t>
+  </si>
+  <si>
+    <t>Licencias de Alcohol</t>
+  </si>
+  <si>
+    <t>Total  General</t>
+  </si>
+  <si>
+    <t>Con pago confirmado</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">REPORTE DEL SISTEMA </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="18"/>
+        <color theme="5"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">SISCOMFERIA </t>
+    </r>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">REPORTE DEL SISTEMA </t>
     </r>
@@ -108,18 +171,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> (07-03-2024 16:55 hrs.)</t>
+      <t xml:space="preserve"> </t>
     </r>
-  </si>
-  <si>
-    <t>PRODUCTOS ADICIONALES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,8 +241,67 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="28"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -198,6 +320,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -208,10 +348,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -222,6 +363,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -231,8 +375,36 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -567,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A757EDF8-B1E5-4DBE-AD85-3317EEF78B18}">
   <dimension ref="A1:AE2325"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -590,40 +762,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
     </row>
     <row r="2" spans="1:31" s="1" customFormat="1" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>15</v>
+      <c r="A2" s="8" t="s">
+        <v>31</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:31" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -668,25 +840,25 @@
       <c r="N3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="8" t="s">
-        <v>16</v>
+      <c r="O3" s="9" t="s">
+        <v>15</v>
       </c>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-      <c r="AB3" s="8"/>
-      <c r="AC3" s="8"/>
-      <c r="AD3" s="8"/>
-      <c r="AE3" s="8"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="9"/>
+      <c r="AA3" s="9"/>
+      <c r="AB3" s="9"/>
+      <c r="AC3" s="9"/>
+      <c r="AD3" s="9"/>
+      <c r="AE3" s="9"/>
     </row>
     <row r="4" spans="1:31" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
@@ -65713,4 +65885,1473 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79CB97A4-670D-4E0A-A4F6-7554E10F7426}">
+  <dimension ref="A1:T58"/>
+  <sheetViews>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection sqref="A1:T1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+    </row>
+    <row r="2" spans="1:20" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+    </row>
+    <row r="3" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="S3" s="12"/>
+      <c r="T3" s="12"/>
+    </row>
+    <row r="4" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+    </row>
+    <row r="5" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+    </row>
+    <row r="6" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="14"/>
+    </row>
+    <row r="7" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+    </row>
+    <row r="8" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
+    </row>
+    <row r="9" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14"/>
+    </row>
+    <row r="10" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="14"/>
+    </row>
+    <row r="11" spans="1:20" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="14"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="14"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="S16" s="12"/>
+      <c r="T16" s="12"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="14"/>
+      <c r="S17" s="14"/>
+      <c r="T17" s="14"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="14"/>
+      <c r="S19" s="14"/>
+      <c r="T19" s="14"/>
+    </row>
+    <row r="20" spans="1:20" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="11"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="S21" s="12"/>
+      <c r="T21" s="12"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="14"/>
+      <c r="S22" s="14"/>
+      <c r="T22" s="14"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+      <c r="R23" s="14"/>
+      <c r="S23" s="14"/>
+      <c r="T23" s="14"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="13"/>
+      <c r="R24" s="14"/>
+      <c r="S24" s="14"/>
+      <c r="T24" s="14"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="12"/>
+      <c r="R25" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="S25" s="12"/>
+      <c r="T25" s="12"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="13"/>
+      <c r="P26" s="13"/>
+      <c r="Q26" s="13"/>
+      <c r="R26" s="14"/>
+      <c r="S26" s="14"/>
+      <c r="T26" s="14"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="14"/>
+      <c r="S27" s="14"/>
+      <c r="T27" s="14"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="13"/>
+      <c r="R28" s="14"/>
+      <c r="S28" s="14"/>
+      <c r="T28" s="14"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="N29" s="16"/>
+      <c r="O29" s="16"/>
+      <c r="P29" s="16"/>
+      <c r="Q29" s="17"/>
+      <c r="R29" s="17"/>
+      <c r="S29" s="17"/>
+      <c r="T29" s="17"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="16"/>
+      <c r="O30" s="16"/>
+      <c r="P30" s="16"/>
+      <c r="Q30" s="17"/>
+      <c r="R30" s="17"/>
+      <c r="S30" s="17"/>
+      <c r="T30" s="17"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A31" s="15"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="16"/>
+      <c r="O31" s="16"/>
+      <c r="P31" s="16"/>
+      <c r="Q31" s="17"/>
+      <c r="R31" s="17"/>
+      <c r="S31" s="17"/>
+      <c r="T31" s="17"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A32" s="15"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="N32" s="16"/>
+      <c r="O32" s="16"/>
+      <c r="P32" s="16"/>
+      <c r="Q32" s="17"/>
+      <c r="R32" s="17"/>
+      <c r="S32" s="17"/>
+      <c r="T32" s="17"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A33" s="15"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="16"/>
+      <c r="N33" s="16"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="16"/>
+      <c r="Q33" s="17"/>
+      <c r="R33" s="17"/>
+      <c r="S33" s="17"/>
+      <c r="T33" s="17"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A34" s="15"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="16"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="16"/>
+      <c r="Q34" s="17"/>
+      <c r="R34" s="17"/>
+      <c r="S34" s="17"/>
+      <c r="T34" s="17"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A36" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="P36" s="12"/>
+      <c r="Q36" s="12"/>
+      <c r="R36" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="S36" s="12"/>
+      <c r="T36" s="12"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
+      <c r="N37" s="10"/>
+      <c r="O37" s="13"/>
+      <c r="P37" s="13"/>
+      <c r="Q37" s="13"/>
+      <c r="R37" s="14"/>
+      <c r="S37" s="14"/>
+      <c r="T37" s="14"/>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="10"/>
+      <c r="N38" s="10"/>
+      <c r="O38" s="13"/>
+      <c r="P38" s="13"/>
+      <c r="Q38" s="13"/>
+      <c r="R38" s="14"/>
+      <c r="S38" s="14"/>
+      <c r="T38" s="14"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="14"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="10"/>
+      <c r="M39" s="10"/>
+      <c r="N39" s="10"/>
+      <c r="O39" s="13"/>
+      <c r="P39" s="13"/>
+      <c r="Q39" s="13"/>
+      <c r="R39" s="14"/>
+      <c r="S39" s="14"/>
+      <c r="T39" s="14"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I40" s="12"/>
+      <c r="J40" s="12"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="10"/>
+      <c r="N40" s="10"/>
+      <c r="O40" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="P40" s="12"/>
+      <c r="Q40" s="12"/>
+      <c r="R40" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="S40" s="12"/>
+      <c r="T40" s="12"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="14"/>
+      <c r="K41" s="10"/>
+      <c r="L41" s="10"/>
+      <c r="M41" s="10"/>
+      <c r="N41" s="10"/>
+      <c r="O41" s="13"/>
+      <c r="P41" s="13"/>
+      <c r="Q41" s="13"/>
+      <c r="R41" s="14"/>
+      <c r="S41" s="14"/>
+      <c r="T41" s="14"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A42" s="10"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="10"/>
+      <c r="L42" s="10"/>
+      <c r="M42" s="10"/>
+      <c r="N42" s="10"/>
+      <c r="O42" s="13"/>
+      <c r="P42" s="13"/>
+      <c r="Q42" s="13"/>
+      <c r="R42" s="14"/>
+      <c r="S42" s="14"/>
+      <c r="T42" s="14"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14"/>
+      <c r="K43" s="10"/>
+      <c r="L43" s="10"/>
+      <c r="M43" s="10"/>
+      <c r="N43" s="10"/>
+      <c r="O43" s="13"/>
+      <c r="P43" s="13"/>
+      <c r="Q43" s="13"/>
+      <c r="R43" s="14"/>
+      <c r="S43" s="14"/>
+      <c r="T43" s="14"/>
+    </row>
+    <row r="44" spans="1:20" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="6"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="11"/>
+      <c r="M44" s="11"/>
+      <c r="N44" s="11"/>
+      <c r="O44" s="11"/>
+      <c r="P44" s="11"/>
+      <c r="Q44" s="11"/>
+      <c r="R44" s="11"/>
+      <c r="S44" s="11"/>
+      <c r="T44" s="11"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A45" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B45" s="18"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I45" s="12"/>
+      <c r="J45" s="12"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="11"/>
+      <c r="M45" s="11"/>
+      <c r="N45" s="11"/>
+      <c r="O45" s="11"/>
+      <c r="P45" s="11"/>
+      <c r="Q45" s="11"/>
+      <c r="R45" s="11"/>
+      <c r="S45" s="11"/>
+      <c r="T45" s="11"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A46" s="18"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="14"/>
+      <c r="J46" s="14"/>
+      <c r="K46" s="11"/>
+      <c r="L46" s="11"/>
+      <c r="M46" s="11"/>
+      <c r="N46" s="11"/>
+      <c r="O46" s="11"/>
+      <c r="P46" s="11"/>
+      <c r="Q46" s="11"/>
+      <c r="R46" s="11"/>
+      <c r="S46" s="11"/>
+      <c r="T46" s="11"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A47" s="18"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14"/>
+      <c r="J47" s="14"/>
+      <c r="K47" s="11"/>
+      <c r="L47" s="11"/>
+      <c r="M47" s="11"/>
+      <c r="N47" s="11"/>
+      <c r="O47" s="11"/>
+      <c r="P47" s="11"/>
+      <c r="Q47" s="11"/>
+      <c r="R47" s="11"/>
+      <c r="S47" s="11"/>
+      <c r="T47" s="11"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A48" s="18"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="14"/>
+      <c r="J48" s="14"/>
+      <c r="K48" s="11"/>
+      <c r="L48" s="11"/>
+      <c r="M48" s="11"/>
+      <c r="N48" s="11"/>
+      <c r="O48" s="11"/>
+      <c r="P48" s="11"/>
+      <c r="Q48" s="11"/>
+      <c r="R48" s="11"/>
+      <c r="S48" s="11"/>
+      <c r="T48" s="11"/>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A49" s="18"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I49" s="12"/>
+      <c r="J49" s="12"/>
+      <c r="K49" s="11"/>
+      <c r="L49" s="11"/>
+      <c r="M49" s="11"/>
+      <c r="N49" s="11"/>
+      <c r="O49" s="11"/>
+      <c r="P49" s="11"/>
+      <c r="Q49" s="11"/>
+      <c r="R49" s="11"/>
+      <c r="S49" s="11"/>
+      <c r="T49" s="11"/>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A50" s="18"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="14"/>
+      <c r="J50" s="14"/>
+      <c r="K50" s="11"/>
+      <c r="L50" s="11"/>
+      <c r="M50" s="11"/>
+      <c r="N50" s="11"/>
+      <c r="O50" s="11"/>
+      <c r="P50" s="11"/>
+      <c r="Q50" s="11"/>
+      <c r="R50" s="11"/>
+      <c r="S50" s="11"/>
+      <c r="T50" s="11"/>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A51" s="18"/>
+      <c r="B51" s="18"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="14"/>
+      <c r="K51" s="11"/>
+      <c r="L51" s="11"/>
+      <c r="M51" s="11"/>
+      <c r="N51" s="11"/>
+      <c r="O51" s="11"/>
+      <c r="P51" s="11"/>
+      <c r="Q51" s="11"/>
+      <c r="R51" s="11"/>
+      <c r="S51" s="11"/>
+      <c r="T51" s="11"/>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A52" s="18"/>
+      <c r="B52" s="18"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="14"/>
+      <c r="J52" s="14"/>
+      <c r="K52" s="11"/>
+      <c r="L52" s="11"/>
+      <c r="M52" s="11"/>
+      <c r="N52" s="11"/>
+      <c r="O52" s="11"/>
+      <c r="P52" s="11"/>
+      <c r="Q52" s="11"/>
+      <c r="R52" s="11"/>
+      <c r="S52" s="11"/>
+      <c r="T52" s="11"/>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A53" s="15"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="15"/>
+      <c r="I53" s="15"/>
+      <c r="J53" s="15"/>
+      <c r="K53" s="15"/>
+      <c r="L53" s="15"/>
+      <c r="M53" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="N53" s="16"/>
+      <c r="O53" s="16"/>
+      <c r="P53" s="16"/>
+      <c r="Q53" s="17"/>
+      <c r="R53" s="17"/>
+      <c r="S53" s="17"/>
+      <c r="T53" s="17"/>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A54" s="15"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="15"/>
+      <c r="J54" s="15"/>
+      <c r="K54" s="15"/>
+      <c r="L54" s="15"/>
+      <c r="M54" s="16"/>
+      <c r="N54" s="16"/>
+      <c r="O54" s="16"/>
+      <c r="P54" s="16"/>
+      <c r="Q54" s="17"/>
+      <c r="R54" s="17"/>
+      <c r="S54" s="17"/>
+      <c r="T54" s="17"/>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A55" s="15"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="15"/>
+      <c r="J55" s="15"/>
+      <c r="K55" s="15"/>
+      <c r="L55" s="15"/>
+      <c r="M55" s="16"/>
+      <c r="N55" s="16"/>
+      <c r="O55" s="16"/>
+      <c r="P55" s="16"/>
+      <c r="Q55" s="17"/>
+      <c r="R55" s="17"/>
+      <c r="S55" s="17"/>
+      <c r="T55" s="17"/>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A56" s="15"/>
+      <c r="B56" s="15"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="15"/>
+      <c r="G56" s="15"/>
+      <c r="H56" s="15"/>
+      <c r="I56" s="15"/>
+      <c r="J56" s="15"/>
+      <c r="K56" s="15"/>
+      <c r="L56" s="15"/>
+      <c r="M56" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="N56" s="16"/>
+      <c r="O56" s="16"/>
+      <c r="P56" s="16"/>
+      <c r="Q56" s="17"/>
+      <c r="R56" s="17"/>
+      <c r="S56" s="17"/>
+      <c r="T56" s="17"/>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A57" s="15"/>
+      <c r="B57" s="15"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="15"/>
+      <c r="G57" s="15"/>
+      <c r="H57" s="15"/>
+      <c r="I57" s="15"/>
+      <c r="J57" s="15"/>
+      <c r="K57" s="15"/>
+      <c r="L57" s="15"/>
+      <c r="M57" s="16"/>
+      <c r="N57" s="16"/>
+      <c r="O57" s="16"/>
+      <c r="P57" s="16"/>
+      <c r="Q57" s="17"/>
+      <c r="R57" s="17"/>
+      <c r="S57" s="17"/>
+      <c r="T57" s="17"/>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A58" s="15"/>
+      <c r="B58" s="15"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="15"/>
+      <c r="G58" s="15"/>
+      <c r="H58" s="15"/>
+      <c r="I58" s="15"/>
+      <c r="J58" s="15"/>
+      <c r="K58" s="15"/>
+      <c r="L58" s="15"/>
+      <c r="M58" s="16"/>
+      <c r="N58" s="16"/>
+      <c r="O58" s="16"/>
+      <c r="P58" s="16"/>
+      <c r="Q58" s="17"/>
+      <c r="R58" s="17"/>
+      <c r="S58" s="17"/>
+      <c r="T58" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="96">
+    <mergeCell ref="A29:L34"/>
+    <mergeCell ref="M53:P55"/>
+    <mergeCell ref="Q53:T55"/>
+    <mergeCell ref="M56:P58"/>
+    <mergeCell ref="Q56:T58"/>
+    <mergeCell ref="K44:T52"/>
+    <mergeCell ref="A53:L58"/>
+    <mergeCell ref="M29:P31"/>
+    <mergeCell ref="Q29:T31"/>
+    <mergeCell ref="M32:P34"/>
+    <mergeCell ref="Q32:T34"/>
+    <mergeCell ref="A45:D52"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E46:G48"/>
+    <mergeCell ref="H46:J48"/>
+    <mergeCell ref="R40:T40"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="H49:J49"/>
+    <mergeCell ref="E50:G52"/>
+    <mergeCell ref="H50:J52"/>
+    <mergeCell ref="K36:N43"/>
+    <mergeCell ref="O41:Q43"/>
+    <mergeCell ref="R41:T43"/>
+    <mergeCell ref="A36:D43"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="E37:G39"/>
+    <mergeCell ref="H37:J39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="E41:G43"/>
+    <mergeCell ref="H41:J43"/>
+    <mergeCell ref="O36:Q36"/>
+    <mergeCell ref="R36:T36"/>
+    <mergeCell ref="O37:Q39"/>
+    <mergeCell ref="R37:T39"/>
+    <mergeCell ref="O40:Q40"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="O4:Q6"/>
+    <mergeCell ref="R4:T6"/>
+    <mergeCell ref="A3:D10"/>
+    <mergeCell ref="E8:G10"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E4:G6"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="O7:Q7"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="O8:Q10"/>
+    <mergeCell ref="R8:T10"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="H8:J10"/>
+    <mergeCell ref="H4:J6"/>
+    <mergeCell ref="K3:N10"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="O17:Q19"/>
+    <mergeCell ref="A11:T11"/>
+    <mergeCell ref="E17:G19"/>
+    <mergeCell ref="H17:J19"/>
+    <mergeCell ref="O12:Q12"/>
+    <mergeCell ref="R12:T12"/>
+    <mergeCell ref="O13:Q15"/>
+    <mergeCell ref="R13:T15"/>
+    <mergeCell ref="O16:Q16"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="E13:G15"/>
+    <mergeCell ref="H13:J15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="E26:G28"/>
+    <mergeCell ref="H26:J28"/>
+    <mergeCell ref="E22:G24"/>
+    <mergeCell ref="H22:J24"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="H25:J25"/>
+    <mergeCell ref="K12:N19"/>
+    <mergeCell ref="A20:T20"/>
+    <mergeCell ref="K21:N28"/>
+    <mergeCell ref="O21:Q21"/>
+    <mergeCell ref="R21:T21"/>
+    <mergeCell ref="O22:Q24"/>
+    <mergeCell ref="R22:T24"/>
+    <mergeCell ref="O25:Q25"/>
+    <mergeCell ref="R25:T25"/>
+    <mergeCell ref="O26:Q28"/>
+    <mergeCell ref="R26:T28"/>
+    <mergeCell ref="A21:D28"/>
+    <mergeCell ref="R17:T19"/>
+    <mergeCell ref="A12:D19"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="H21:J21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>